<commit_message>
Updates Reception perception data
</commit_message>
<xml_diff>
--- a/data/common/Reception_Perception_Rookies.xlsx
+++ b/data/common/Reception_Perception_Rookies.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/28a1ee50a88aa706/python_work/Dynasty_tools/data/common/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="232" documentId="8_{7BA15C0B-EFF0-4E59-B702-89E2371692A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6B26462C-CB72-42CF-A37D-A38E605CF4EE}"/>
+  <xr:revisionPtr revIDLastSave="260" documentId="8_{7BA15C0B-EFF0-4E59-B702-89E2371692A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C38FF8ED-14EB-41E3-A325-469F1223F58B}"/>
   <bookViews>
-    <workbookView xWindow="1520" yWindow="1520" windowWidth="28800" windowHeight="15460" xr2:uid="{CF82EDE9-4597-4981-98B9-E15CE2DB7798}"/>
+    <workbookView xWindow="700" yWindow="12290" windowWidth="20840" windowHeight="15460" xr2:uid="{CF82EDE9-4597-4981-98B9-E15CE2DB7798}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="95">
   <si>
     <t>Player</t>
   </si>
@@ -586,6 +586,33 @@
 Upside: Minimal. His best-case scenario is likely becoming a low-volume, reception-dependent player useful only in very deep PPR leagues, contingent on finding that ideal niche role.
 Downside: Extremely high. His size makes him a major injury risk, and his inability to beat man/press coverage or create YAC likely keeps him off the field or limits him to a handful of targets per game even if active.
 As a likely late Day 3 pick or UDFA, Johnson should be avoided in most dynasty rookie drafts. He lacks the necessary tools to overcome his unprecedented physical limitations for consistent fantasy production.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Shows flashes of good routes and YAC skills but needs development and early role-catering.	</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Love this guy. Beats man and zone. Dominant underneath. Catches everything, breaks tackles.	</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Impressive route runner who projects well as a flanker. Attacks the ball and wins on in-breakers.	</t>
+  </si>
+  <si>
+    <t xml:space="preserve">I can easily see him being a useful popgun slot receiver in the league but limited player.	</t>
+  </si>
+  <si>
+    <t xml:space="preserve">He's ranked this low as a pure wide receiver but I think he can be more useful in a gadget role.	</t>
+  </si>
+  <si>
+    <t>The Rest</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Solid zone-beater but struggles to win against man coverage given lack of size and speed.	</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Will be a 26-year-old rookie but shows some ability to translate into a big slot role.	</t>
+  </si>
+  <si>
+    <t xml:space="preserve">I can see him developing into a reliable slot, flanker rotation guy at some point. Has some game.	</t>
   </si>
 </sst>
 </file>
@@ -643,10 +670,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -968,8 +991,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B70176A1-B136-4145-B48A-7863F0F59492}">
   <dimension ref="A1:R67"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="S18" sqref="S18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A19" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1580,6 +1604,15 @@
       <c r="D12" s="3" t="s">
         <v>75</v>
       </c>
+      <c r="E12" s="3">
+        <v>61</v>
+      </c>
+      <c r="F12" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="G12" s="3" t="s">
+        <v>86</v>
+      </c>
       <c r="H12">
         <v>49.4</v>
       </c>
@@ -1627,6 +1660,12 @@
       <c r="D13" t="s">
         <v>69</v>
       </c>
+      <c r="F13" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="G13" s="3" t="s">
+        <v>87</v>
+      </c>
       <c r="H13">
         <v>53</v>
       </c>
@@ -1671,6 +1710,15 @@
       <c r="D14" t="s">
         <v>72</v>
       </c>
+      <c r="E14" s="3">
+        <v>37</v>
+      </c>
+      <c r="F14" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="G14" s="3" t="s">
+        <v>88</v>
+      </c>
       <c r="H14">
         <v>47.8</v>
       </c>
@@ -1718,6 +1766,15 @@
       <c r="D15" t="s">
         <v>76</v>
       </c>
+      <c r="E15" s="3">
+        <v>73</v>
+      </c>
+      <c r="F15" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="G15" s="3" t="s">
+        <v>89</v>
+      </c>
       <c r="H15">
         <v>45.8</v>
       </c>
@@ -1760,12 +1817,21 @@
         <v>3</v>
       </c>
     </row>
-    <row r="17" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:18" ht="87" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>18</v>
       </c>
       <c r="B17" t="s">
         <v>3</v>
+      </c>
+      <c r="E17" s="3">
+        <v>87</v>
+      </c>
+      <c r="F17" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="G17" s="3" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="18" spans="1:18" ht="409.5" x14ac:dyDescent="0.35">
@@ -1781,6 +1847,15 @@
       <c r="D18" t="s">
         <v>82</v>
       </c>
+      <c r="E18" s="3">
+        <v>75</v>
+      </c>
+      <c r="F18" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="G18" s="3" t="s">
+        <v>92</v>
+      </c>
       <c r="H18">
         <v>42.1</v>
       </c>
@@ -1862,20 +1937,38 @@
         <v>50</v>
       </c>
     </row>
-    <row r="20" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:18" ht="87" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>21</v>
       </c>
       <c r="B20" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="21" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="E20" s="3">
+        <v>78</v>
+      </c>
+      <c r="F20" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="G20" s="3" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="21" spans="1:18" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>22</v>
       </c>
       <c r="B21" t="s">
         <v>3</v>
+      </c>
+      <c r="E21">
+        <v>83</v>
+      </c>
+      <c r="F21" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="G21" s="3" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="27" spans="1:18" x14ac:dyDescent="0.35">

</xml_diff>